<commit_message>
Quick edits to see how code works
</commit_message>
<xml_diff>
--- a/clocking.xlsx
+++ b/clocking.xlsx
@@ -14,45 +14,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
   <si>
-    <t>8FD8ADBD20</t>
+    <t>Freddy Velez</t>
   </si>
   <si>
-    <t>IN -&gt; 2017/01/31 18:57</t>
+    <t>4FD889D140</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/13 18:45</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="General" numFmtId="164"/>
-  </numFmts>
-  <fonts count="4">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
       <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <color rgb="00000000"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <color rgb="00000000"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <color rgb="00000000"/>
+      <color rgb="FF000000"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -73,27 +56,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+  <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="7" name="Currency [0]" xfId="0"/>
-    <cellStyle builtinId="5" name="Percent" xfId="1"/>
-    <cellStyle builtinId="4" name="Currency" xfId="2"/>
-    <cellStyle builtinId="3" name="Comma" xfId="3"/>
-    <cellStyle builtinId="0" name="Normal" xfId="4"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="5"/>
+  <cellStyles count="1">
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -385,42 +356,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:A3"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A11" activeCellId="0" pane="topLeft" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="A13" sqref="A1:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="40"/>
+    <col customWidth="1" max="4" min="1" style="1" width="40"/>
     <col customWidth="1" max="1" min="1" style="1" width="40"/>
     <col customWidth="1" max="2" min="2" style="1" width="40"/>
-    <col customWidth="1" max="2" min="2" style="1" width="40"/>
     <col customWidth="1" max="3" min="3" style="1" width="40"/>
-    <col customWidth="1" max="3" min="3" style="1" width="40"/>
-    <col customWidth="1" max="4" min="4" style="1" width="40"/>
     <col customWidth="1" max="4" min="4" style="1" width="40"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" useFirstPageNumber="1" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;K000000&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;K000000Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Updated code to remove some typos
</commit_message>
<xml_diff>
--- a/clocking.xlsx
+++ b/clocking.xlsx
@@ -14,12 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
-    <t>8FD8ADBD20</t>
+    <t>Freddy Velez</t>
+  </si>
+  <si>
+    <t>4FD889D140</t>
   </si>
   <si>
     <t>IN -&gt; 2017/01/31 18:57</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/14 17:22</t>
   </si>
 </sst>
 </file>
@@ -74,11 +80,11 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
@@ -88,11 +94,11 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="7" name="Currency [0]" xfId="0"/>
-    <cellStyle builtinId="5" name="Percent" xfId="1"/>
-    <cellStyle builtinId="4" name="Currency" xfId="2"/>
-    <cellStyle builtinId="3" name="Comma" xfId="3"/>
-    <cellStyle builtinId="0" name="Normal" xfId="4"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="1"/>
+    <cellStyle builtinId="5" name="Percent" xfId="2"/>
+    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="3" name="Comma" xfId="4"/>
     <cellStyle builtinId="6" name="Comma [0]" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -389,7 +395,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A2:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A11" activeCellId="0" pane="topLeft" sqref="A11"/>
@@ -407,14 +413,24 @@
     <col customWidth="1" max="4" min="4" style="1" width="40"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bugs in timer.py file
</commit_message>
<xml_diff>
--- a/clocking.xlsx
+++ b/clocking.xlsx
@@ -14,18 +14,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>Freddy Velez</t>
   </si>
   <si>
+    <t>John Tomanelli</t>
+  </si>
+  <si>
     <t>4FD889D140</t>
   </si>
   <si>
+    <t>CFD89370C0</t>
+  </si>
+  <si>
     <t>IN -&gt; 2017/01/31 18:57</t>
   </si>
   <si>
+    <t>IN -&gt; 2017/02/15 14:46</t>
+  </si>
+  <si>
     <t>OUT -&gt; 2017/02/14 17:22</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/15 14:47</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/14 17:26</t>
   </si>
 </sst>
 </file>
@@ -395,7 +410,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A11" activeCellId="0" pane="topLeft" sqref="A11"/>
@@ -413,24 +428,41 @@
     <col customWidth="1" max="4" min="4" style="1" width="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified code to run using Python3
</commit_message>
<xml_diff>
--- a/clocking.xlsx
+++ b/clocking.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr codeName="ThisWorkbook"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr codeName="ThisWorkbook"/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>Freddy Velez</t>
   </si>
@@ -41,6 +41,36 @@
   </si>
   <si>
     <t>IN -&gt; 2017/02/14 17:26</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/15 15:03</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/15 15:03</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/18 14:33</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/18 14:35</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/18 14:35</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/18 14:37</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/18 14:37</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/18 14:38</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/02/18 14:41</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/02/18 14:41</t>
   </si>
 </sst>
 </file>
@@ -95,18 +125,18 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -116,7 +146,6 @@
     <cellStyle builtinId="3" name="Comma" xfId="4"/>
     <cellStyle builtinId="6" name="Comma [0]" xfId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
@@ -410,13 +439,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A11" activeCellId="0" pane="topLeft" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="1" width="40"/>
     <col customWidth="1" max="1" min="1" style="1" width="40"/>
@@ -465,6 +494,61 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
@@ -472,6 +556,10 @@
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;K000000&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;K000000Page &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>